<commit_message>
Webscrapping de multiplas listas de trilhas e cursos
</commit_message>
<xml_diff>
--- a/data/trilhas_atualizadas.xlsx
+++ b/data/trilhas_atualizadas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,10 +516,64 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://app.datacamp.com/learn/career-tracks/associate-data-scientist--in-python</t>
+          <t>https://app.datacamp.com/learn/career-tracks/associate-data-scientist-in-python</t>
         </is>
       </c>
       <c r="D5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Excel Fundamentals</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/excel-fundamentals</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Git Fundamentals</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/git-fundamentals</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SQL Fundamentals</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://app.datacamp.com/learn/career-tracks/sql-fundamentals</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>